<commit_message>
minimized c array to 500lines
</commit_message>
<xml_diff>
--- a/BB Regression.xlsx
+++ b/BB Regression.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\my_BBTF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GithubProjects\Bounding_Box_Regression_TF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7EF8391-4F5C-4787-9E03-660B6ADA88B3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811E5D46-7843-40DA-8F3C-252901FF0814}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DAA3E04F-96D0-46C7-B302-9D6FE4DA4CAC}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DAA3E04F-96D0-46C7-B302-9D6FE4DA4CAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Description</t>
   </si>
@@ -160,6 +160,21 @@
   </si>
   <si>
     <t>iou 0.8718</t>
+  </si>
+  <si>
+    <t>still too large, minimize more</t>
+  </si>
+  <si>
+    <t>issue is after conversion to c array took too much space</t>
+  </si>
+  <si>
+    <t>IoU 0.8545</t>
+  </si>
+  <si>
+    <t>Even more</t>
+  </si>
+  <si>
+    <t>IoU 0.8495</t>
   </si>
 </sst>
 </file>
@@ -300,6 +315,94 @@
         <a:xfrm>
           <a:off x="0" y="11887200"/>
           <a:ext cx="3680779" cy="4831499"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3673150</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>23183</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5293EFA-4903-42A1-8E00-1AA8E2E4F7C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="99060" y="17693640"/>
+          <a:ext cx="3574090" cy="3726503"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3551228</xdr:colOff>
+      <xdr:row>141</xdr:row>
+      <xdr:rowOff>107003</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92CC5472-207E-4505-87E8-F2FDA72A1CC7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="21897975"/>
+          <a:ext cx="3551228" cy="3726503"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -608,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AC5A132-BC5E-461D-9F3B-DBD88F5A6862}">
-  <dimension ref="A1:L94"/>
+  <dimension ref="A1:L143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="G123" sqref="G123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1232,9 +1335,32 @@
         <v>41</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>43</v>
+      </c>
+      <c r="B96" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
issue with ram size esp8266
</commit_message>
<xml_diff>
--- a/BB Regression.xlsx
+++ b/BB Regression.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GithubProjects\Bounding_Box_Regression_TF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\my_BBTF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811E5D46-7843-40DA-8F3C-252901FF0814}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4965708-9003-406C-83ED-41B0FCA41F67}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DAA3E04F-96D0-46C7-B302-9D6FE4DA4CAC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DAA3E04F-96D0-46C7-B302-9D6FE4DA4CAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>Description</t>
   </si>
@@ -175,6 +175,24 @@
   </si>
   <si>
     <t>IoU 0.8495</t>
+  </si>
+  <si>
+    <t>Sketch uses 177248 bytes (18%) of program storage space. Maximum is 983040 bytes.</t>
+  </si>
+  <si>
+    <t>Global variables use 121480 bytes (46%) of dynamic memory, leaving 140664 bytes for local variables. Maximum is 262144 bytes.</t>
+  </si>
+  <si>
+    <t>In Nano 33 BLE</t>
+  </si>
+  <si>
+    <t>In nodemcu</t>
+  </si>
+  <si>
+    <t>Sketch uses 372460 bytes (35%) of program storage space. Maximum is 1044464 bytes.</t>
+  </si>
+  <si>
+    <t>Global variables use 69728 bytes (85%) of dynamic memory, leaving 12192 bytes for local variables. Maximum is 81920 bytes.</t>
   </si>
 </sst>
 </file>
@@ -711,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AC5A132-BC5E-461D-9F3B-DBD88F5A6862}">
-  <dimension ref="A1:L143"/>
+  <dimension ref="A1:L157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="G123" sqref="G123"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="A158" sqref="A158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1363,6 +1381,48 @@
         <v>47</v>
       </c>
     </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <f>81920-69728</f>
+        <v>12192</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A157">
+        <f>12192/1024</f>
+        <v>11.90625</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
new model, arduino done
</commit_message>
<xml_diff>
--- a/BB Regression.xlsx
+++ b/BB Regression.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\my_BBTF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4965708-9003-406C-83ED-41B0FCA41F67}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA86789E-9E9B-43BD-A563-EC2CC521F5F5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DAA3E04F-96D0-46C7-B302-9D6FE4DA4CAC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{DAA3E04F-96D0-46C7-B302-9D6FE4DA4CAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>Description</t>
   </si>
@@ -177,22 +177,13 @@
     <t>IoU 0.8495</t>
   </si>
   <si>
-    <t>Sketch uses 177248 bytes (18%) of program storage space. Maximum is 983040 bytes.</t>
-  </si>
-  <si>
-    <t>Global variables use 121480 bytes (46%) of dynamic memory, leaving 140664 bytes for local variables. Maximum is 262144 bytes.</t>
-  </si>
-  <si>
-    <t>In Nano 33 BLE</t>
-  </si>
-  <si>
-    <t>In nodemcu</t>
-  </si>
-  <si>
-    <t>Sketch uses 372460 bytes (35%) of program storage space. Maximum is 1044464 bytes.</t>
-  </si>
-  <si>
-    <t>Global variables use 69728 bytes (85%) of dynamic memory, leaving 12192 bytes for local variables. Maximum is 81920 bytes.</t>
+    <t>Sketch uses 307528 bytes (29%) of program storage space. Maximum is 1044464 bytes.</t>
+  </si>
+  <si>
+    <t>Global variables use 67412 bytes (82%) of dynamic memory, leaving 14508 bytes for local variables. Maximum is 81920 bytes.</t>
+  </si>
+  <si>
+    <t>in nodemcu</t>
   </si>
 </sst>
 </file>
@@ -729,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AC5A132-BC5E-461D-9F3B-DBD88F5A6862}">
-  <dimension ref="A1:L157"/>
+  <dimension ref="A1:L147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="A158" sqref="A158"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1381,46 +1372,19 @@
         <v>47</v>
       </c>
     </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A148" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A151" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A152" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A153" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A156">
-        <f>81920-69728</f>
-        <v>12192</v>
-      </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A157">
-        <f>12192/1024</f>
-        <v>11.90625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed to arduino ble
</commit_message>
<xml_diff>
--- a/BB Regression.xlsx
+++ b/BB Regression.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\my_BBTF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA86789E-9E9B-43BD-A563-EC2CC521F5F5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7644D8FF-5DE9-4070-AF36-4FB485233622}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{DAA3E04F-96D0-46C7-B302-9D6FE4DA4CAC}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>Description</t>
   </si>
@@ -184,6 +184,15 @@
   </si>
   <si>
     <t>in nodemcu</t>
+  </si>
+  <si>
+    <t>Sketch uses 120424 bytes (12%) of program storage space. Maximum is 983040 bytes.</t>
+  </si>
+  <si>
+    <t>Global variables use 69128 bytes (26%) of dynamic memory, leaving 193016 bytes for local variables. Maximum is 262144 bytes.</t>
+  </si>
+  <si>
+    <t>in arduino (store image in ram)</t>
   </si>
 </sst>
 </file>
@@ -720,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AC5A132-BC5E-461D-9F3B-DBD88F5A6862}">
-  <dimension ref="A1:L147"/>
+  <dimension ref="A1:L151"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="A146" sqref="A146"/>
+      <selection activeCell="A149" sqref="A149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1387,6 +1396,21 @@
         <v>49</v>
       </c>
     </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
fix data type error
</commit_message>
<xml_diff>
--- a/BB Regression.xlsx
+++ b/BB Regression.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\my_BBTF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GithubProjects\Bounding_Box_Regression_TF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7644D8FF-5DE9-4070-AF36-4FB485233622}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05AA33AD-3E02-4C55-B494-60F75D78A7F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{DAA3E04F-96D0-46C7-B302-9D6FE4DA4CAC}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DAA3E04F-96D0-46C7-B302-9D6FE4DA4CAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -262,7 +262,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>282341</xdr:colOff>
+      <xdr:colOff>286151</xdr:colOff>
       <xdr:row>60</xdr:row>
       <xdr:rowOff>483</xdr:rowOff>
     </xdr:to>
@@ -306,7 +306,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>3680779</xdr:colOff>
+      <xdr:colOff>3676969</xdr:colOff>
       <xdr:row>91</xdr:row>
       <xdr:rowOff>76619</xdr:rowOff>
     </xdr:to>
@@ -350,9 +350,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>3673150</xdr:colOff>
+      <xdr:colOff>3676960</xdr:colOff>
       <xdr:row>117</xdr:row>
-      <xdr:rowOff>23183</xdr:rowOff>
+      <xdr:rowOff>19373</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -394,9 +394,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>3551228</xdr:colOff>
+      <xdr:colOff>3558848</xdr:colOff>
       <xdr:row>141</xdr:row>
-      <xdr:rowOff>107003</xdr:rowOff>
+      <xdr:rowOff>101288</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -732,7 +732,7 @@
   <dimension ref="A1:L151"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="A149" sqref="A149"/>
+      <selection activeCell="J145" sqref="J145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>